<commit_message>
+  rolling window 5 years
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -412,16 +412,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.4642857142857143</v>
+        <v>0.4625</v>
       </c>
       <c r="C2">
-        <v>0.9935586282185146</v>
+        <v>0.9518662492434183</v>
       </c>
       <c r="D2">
-        <v>0.51171875</v>
+        <v>0.53125</v>
       </c>
       <c r="E2">
-        <v>0.8862810581922531</v>
+        <v>0.8463120460510254</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -429,16 +429,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5290178571428571</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="C3">
-        <v>0.8268729746341705</v>
+        <v>0.7987846771876017</v>
       </c>
       <c r="D3">
-        <v>0.5546875</v>
+        <v>0.4661458333333333</v>
       </c>
       <c r="E3">
-        <v>0.8109036982059479</v>
+        <v>0.7989378074804941</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -446,16 +446,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5290178571428571</v>
+        <v>0.525</v>
       </c>
       <c r="C4">
-        <v>0.7809640339442662</v>
+        <v>0.7728306333223979</v>
       </c>
       <c r="D4">
-        <v>0.50390625</v>
+        <v>0.4921875</v>
       </c>
       <c r="E4">
-        <v>0.7814773172140121</v>
+        <v>0.7641796668370565</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -463,16 +463,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5345982142857143</v>
+        <v>0.5041666666666667</v>
       </c>
       <c r="C5">
-        <v>0.7569932426725116</v>
+        <v>0.776631768544515</v>
       </c>
       <c r="D5">
-        <v>0.4921875</v>
+        <v>0.5182291666666666</v>
       </c>
       <c r="E5">
-        <v>0.763912096619606</v>
+        <v>0.753129631280899</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -480,16 +480,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5223214285714286</v>
+        <v>0.4927083333333334</v>
       </c>
       <c r="C6">
-        <v>0.7441199805055346</v>
+        <v>0.7653687198956808</v>
       </c>
       <c r="D6">
-        <v>0.51953125</v>
+        <v>0.484375</v>
       </c>
       <c r="E6">
-        <v>0.750432088971138</v>
+        <v>0.7486079931259155</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -497,16 +497,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5435267857142857</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="C7">
-        <v>0.734751603433064</v>
+        <v>0.735435136159261</v>
       </c>
       <c r="D7">
-        <v>0.484375</v>
+        <v>0.4921875</v>
       </c>
       <c r="E7">
-        <v>0.7469728887081146</v>
+        <v>0.7412130236625671</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -514,16 +514,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5279017857142857</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C8">
-        <v>0.7323949337005615</v>
+        <v>0.7463503042856853</v>
       </c>
       <c r="D8">
-        <v>0.4921875</v>
+        <v>0.4375</v>
       </c>
       <c r="E8">
-        <v>0.7397944182157516</v>
+        <v>0.7417400379975637</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -531,16 +531,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5323660714285714</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="C9">
-        <v>0.7283421797411782</v>
+        <v>0.7456873734792073</v>
       </c>
       <c r="D9">
-        <v>0.52734375</v>
+        <v>0.5104166666666666</v>
       </c>
       <c r="E9">
-        <v>0.7353862076997757</v>
+        <v>0.7307079037030538</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -548,16 +548,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5390625</v>
+        <v>0.509375</v>
       </c>
       <c r="C10">
-        <v>0.7237418591976166</v>
+        <v>0.7477637330691019</v>
       </c>
       <c r="D10">
-        <v>0.4921875</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E10">
-        <v>0.7359625250101089</v>
+        <v>0.7338186105092367</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -565,16 +565,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5301339285714286</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C11">
-        <v>0.724291809967586</v>
+        <v>0.7345525662104289</v>
       </c>
       <c r="D11">
-        <v>0.49609375</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E11">
-        <v>0.7320725321769714</v>
+        <v>0.7284386257330576</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -582,16 +582,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.5357142857142857</v>
+        <v>0.5052083333333334</v>
       </c>
       <c r="C12">
-        <v>0.7219931355544499</v>
+        <v>0.744333811601003</v>
       </c>
       <c r="D12">
-        <v>0.48046875</v>
+        <v>0.5442708333333334</v>
       </c>
       <c r="E12">
-        <v>0.7313155680894852</v>
+        <v>0.723228394985199</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -599,16 +599,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5323660714285714</v>
+        <v>0.5010416666666667</v>
       </c>
       <c r="C13">
-        <v>0.7212426832744053</v>
+        <v>0.740562637646993</v>
       </c>
       <c r="D13">
-        <v>0.51171875</v>
+        <v>0.4973958333333333</v>
       </c>
       <c r="E13">
-        <v>0.7287202030420303</v>
+        <v>0.7245149115721384</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -616,16 +616,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.5390625</v>
+        <v>0.5114583333333333</v>
       </c>
       <c r="C14">
-        <v>0.7154522282736642</v>
+        <v>0.734390127658844</v>
       </c>
       <c r="D14">
-        <v>0.4921875</v>
+        <v>0.5182291666666666</v>
       </c>
       <c r="E14">
-        <v>0.7264124602079391</v>
+        <v>0.7235841850439707</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -633,16 +633,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.5401785714285714</v>
+        <v>0.51875</v>
       </c>
       <c r="C15">
-        <v>0.7172403761318752</v>
+        <v>0.7388193845748902</v>
       </c>
       <c r="D15">
-        <v>0.50390625</v>
+        <v>0.4739583333333333</v>
       </c>
       <c r="E15">
-        <v>0.7253462821245193</v>
+        <v>0.7298851013183594</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -650,16 +650,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5457589285714286</v>
+        <v>0.521875</v>
       </c>
       <c r="C16">
-        <v>0.7164215700966972</v>
+        <v>0.7361614425977071</v>
       </c>
       <c r="D16">
-        <v>0.4921875</v>
+        <v>0.5</v>
       </c>
       <c r="E16">
-        <v>0.7253166437149048</v>
+        <v>0.7228529155254364</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -667,16 +667,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.5390625</v>
+        <v>0.521875</v>
       </c>
       <c r="C17">
-        <v>0.7155714801379612</v>
+        <v>0.7301985343297323</v>
       </c>
       <c r="D17">
-        <v>0.5078125</v>
+        <v>0.4765625</v>
       </c>
       <c r="E17">
-        <v>0.7238609045743942</v>
+        <v>0.7311780154705048</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -684,16 +684,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.546875</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="C18">
-        <v>0.7140096894332341</v>
+        <v>0.7257394989331564</v>
       </c>
       <c r="D18">
-        <v>0.53515625</v>
+        <v>0.5026041666666666</v>
       </c>
       <c r="E18">
-        <v>0.721981942653656</v>
+        <v>0.7317436834176382</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -701,16 +701,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5368303571428571</v>
+        <v>0.5072916666666667</v>
       </c>
       <c r="C19">
-        <v>0.7135516617979322</v>
+        <v>0.7388754407564799</v>
       </c>
       <c r="D19">
-        <v>0.51953125</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E19">
-        <v>0.7220138758420944</v>
+        <v>0.722976932922999</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -718,16 +718,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5446428571428571</v>
+        <v>0.515625</v>
       </c>
       <c r="C20">
-        <v>0.7147959768772125</v>
+        <v>0.7305711666742961</v>
       </c>
       <c r="D20">
-        <v>0.54296875</v>
+        <v>0.4609375</v>
       </c>
       <c r="E20">
-        <v>0.7212056517601013</v>
+        <v>0.7322059770425161</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -735,16 +735,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.5524553571428571</v>
+        <v>0.5270833333333333</v>
       </c>
       <c r="C21">
-        <v>0.7138191333838871</v>
+        <v>0.7243668278058369</v>
       </c>
       <c r="D21">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E21">
-        <v>0.7206640839576721</v>
+        <v>0.7356695135434469</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -752,16 +752,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.5446428571428571</v>
+        <v>0.4916666666666666</v>
       </c>
       <c r="C22">
-        <v>0.7106727276529584</v>
+        <v>0.7380374113718668</v>
       </c>
       <c r="D22">
-        <v>0.5078125</v>
+        <v>0.4713541666666667</v>
       </c>
       <c r="E22">
-        <v>0.721645176410675</v>
+        <v>0.7252024710178375</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -769,16 +769,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.5435267857142857</v>
+        <v>0.5239583333333333</v>
       </c>
       <c r="C23">
-        <v>0.710873714515141</v>
+        <v>0.7314259648323059</v>
       </c>
       <c r="D23">
-        <v>0.5078125</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E23">
-        <v>0.7207087725400925</v>
+        <v>0.7349865535895029</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -786,16 +786,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5424107142857143</v>
+        <v>0.5072916666666667</v>
       </c>
       <c r="C24">
-        <v>0.7123693142618451</v>
+        <v>0.7208680987358094</v>
       </c>
       <c r="D24">
-        <v>0.50390625</v>
+        <v>0.484375</v>
       </c>
       <c r="E24">
-        <v>0.7207996994256973</v>
+        <v>0.7260819574197134</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -803,16 +803,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5401785714285714</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="C25">
-        <v>0.7120191412312644</v>
+        <v>0.7252694368362427</v>
       </c>
       <c r="D25">
-        <v>0.49609375</v>
+        <v>0.4921875</v>
       </c>
       <c r="E25">
-        <v>0.7211433351039886</v>
+        <v>0.7283205091953278</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -820,16 +820,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5457589285714286</v>
+        <v>0.5270833333333333</v>
       </c>
       <c r="C26">
-        <v>0.7092399639742715</v>
+        <v>0.7252019643783569</v>
       </c>
       <c r="D26">
-        <v>0.54296875</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E26">
-        <v>0.719385638833046</v>
+        <v>0.7261911233266195</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -837,16 +837,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5379464285714286</v>
+        <v>0.5458333333333333</v>
       </c>
       <c r="C27">
-        <v>0.7103607399123055</v>
+        <v>0.7190420786539714</v>
       </c>
       <c r="D27">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E27">
-        <v>0.7191231697797775</v>
+        <v>0.7550978263219198</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -854,16 +854,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5435267857142857</v>
+        <v>0.4916666666666666</v>
       </c>
       <c r="C28">
-        <v>0.7119489908218384</v>
+        <v>0.7401295900344849</v>
       </c>
       <c r="D28">
-        <v>0.52734375</v>
+        <v>0.4765625</v>
       </c>
       <c r="E28">
-        <v>0.7192712128162384</v>
+        <v>0.7286915977795919</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -871,16 +871,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.5535714285714286</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C29">
-        <v>0.7094197911875588</v>
+        <v>0.7295502265294392</v>
       </c>
       <c r="D29">
-        <v>0.53125</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E29">
-        <v>0.7191309630870819</v>
+        <v>0.7424005270004272</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -888,16 +888,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5401785714285714</v>
+        <v>0.5239583333333333</v>
       </c>
       <c r="C30">
-        <v>0.7094432754176003</v>
+        <v>0.7236273447672527</v>
       </c>
       <c r="D30">
-        <v>0.50390625</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E30">
-        <v>0.7197939306497574</v>
+        <v>0.7371327877044678</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -905,16 +905,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5435267857142857</v>
+        <v>0.5177083333333333</v>
       </c>
       <c r="C31">
-        <v>0.7078987019402641</v>
+        <v>0.7200861930847168</v>
       </c>
       <c r="D31">
-        <v>0.50390625</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E31">
-        <v>0.7208888232707977</v>
+        <v>0.7410170634587606</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -922,16 +922,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5424107142857143</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C32">
-        <v>0.7098526528903416</v>
+        <v>0.7202006697654724</v>
       </c>
       <c r="D32">
-        <v>0.49609375</v>
+        <v>0.4739583333333333</v>
       </c>
       <c r="E32">
-        <v>0.7196145057678223</v>
+        <v>0.7280525465806326</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -939,16 +939,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5290178571428571</v>
+        <v>0.5322916666666667</v>
       </c>
       <c r="C33">
-        <v>0.70976379939488</v>
+        <v>0.7218029697736105</v>
       </c>
       <c r="D33">
-        <v>0.52734375</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E33">
-        <v>0.7187008708715439</v>
+        <v>0.7385540107885996</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -956,16 +956,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5345982142857143</v>
+        <v>0.5458333333333333</v>
       </c>
       <c r="C34">
-        <v>0.7132837814944131</v>
+        <v>0.7142613093058269</v>
       </c>
       <c r="D34">
-        <v>0.50390625</v>
+        <v>0.46875</v>
       </c>
       <c r="E34">
-        <v>0.719655841588974</v>
+        <v>0.7334762215614319</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -973,16 +973,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5379464285714286</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="C35">
-        <v>0.7106244521481651</v>
+        <v>0.723831041653951</v>
       </c>
       <c r="D35">
-        <v>0.5078125</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E35">
-        <v>0.7196044623851776</v>
+        <v>0.7500119705994924</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -990,16 +990,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.5502232142857143</v>
+        <v>0.515625</v>
       </c>
       <c r="C36">
-        <v>0.707237469298499</v>
+        <v>0.7257665673891703</v>
       </c>
       <c r="D36">
-        <v>0.5</v>
+        <v>0.4739583333333333</v>
       </c>
       <c r="E36">
-        <v>0.7199190557003021</v>
+        <v>0.7312738398710886</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1007,16 +1007,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.5502232142857143</v>
+        <v>0.528125</v>
       </c>
       <c r="C37">
-        <v>0.7085717107568469</v>
+        <v>0.722018814086914</v>
       </c>
       <c r="D37">
-        <v>0.50390625</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E37">
-        <v>0.7201875448226929</v>
+        <v>0.7566766242186228</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1024,16 +1024,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5368303571428571</v>
+        <v>0.5302083333333333</v>
       </c>
       <c r="C38">
-        <v>0.7090789973735809</v>
+        <v>0.7160040338834127</v>
       </c>
       <c r="D38">
-        <v>0.53515625</v>
+        <v>0.46875</v>
       </c>
       <c r="E38">
-        <v>0.7181194126605988</v>
+        <v>0.7355140348275503</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1041,16 +1041,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.5401785714285714</v>
+        <v>0.5354166666666667</v>
       </c>
       <c r="C39">
-        <v>0.708601176738739</v>
+        <v>0.7194936990737915</v>
       </c>
       <c r="D39">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E39">
-        <v>0.718305841088295</v>
+        <v>0.7413596709569296</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1058,16 +1058,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5412946428571429</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C40">
-        <v>0.707783158336367</v>
+        <v>0.7202193935712179</v>
       </c>
       <c r="D40">
-        <v>0.5078125</v>
+        <v>0.46875</v>
       </c>
       <c r="E40">
-        <v>0.7194080501794815</v>
+        <v>0.7305180132389069</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1075,16 +1075,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5435267857142857</v>
+        <v>0.5385416666666667</v>
       </c>
       <c r="C41">
-        <v>0.7075308603899819</v>
+        <v>0.7119321227073669</v>
       </c>
       <c r="D41">
-        <v>0.5078125</v>
+        <v>0.4635416666666667</v>
       </c>
       <c r="E41">
-        <v>0.7187818139791489</v>
+        <v>0.7333577573299408</v>
       </c>
     </row>
   </sheetData>
@@ -1119,16 +1119,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.4966517857142857</v>
+        <v>0.475</v>
       </c>
       <c r="C2">
-        <v>0.9207921198436192</v>
+        <v>0.9157173315684001</v>
       </c>
       <c r="D2">
-        <v>0.51953125</v>
+        <v>0.4270833333333333</v>
       </c>
       <c r="E2">
-        <v>0.8404034376144409</v>
+        <v>0.8649795552094778</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1136,16 +1136,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5323660714285714</v>
+        <v>0.4989583333333333</v>
       </c>
       <c r="C3">
-        <v>0.7866621783801487</v>
+        <v>0.7933442115783691</v>
       </c>
       <c r="D3">
-        <v>0.54296875</v>
+        <v>0.4479166666666667</v>
       </c>
       <c r="E3">
-        <v>0.7854975014925003</v>
+        <v>0.8032051424185435</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1153,16 +1153,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5446428571428571</v>
+        <v>0.521875</v>
       </c>
       <c r="C4">
-        <v>0.7575922736099788</v>
+        <v>0.7595261613527934</v>
       </c>
       <c r="D4">
-        <v>0.54296875</v>
+        <v>0.4479166666666667</v>
       </c>
       <c r="E4">
-        <v>0.7617647796869278</v>
+        <v>0.7803545494874319</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1170,16 +1170,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5368303571428571</v>
+        <v>0.509375</v>
       </c>
       <c r="C5">
-        <v>0.7397344708442688</v>
+        <v>0.7642112612724304</v>
       </c>
       <c r="D5">
-        <v>0.54296875</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E5">
-        <v>0.7483324706554413</v>
+        <v>0.7657210429509481</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1187,16 +1187,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5390625</v>
+        <v>0.503125</v>
       </c>
       <c r="C6">
-        <v>0.7328096117292132</v>
+        <v>0.7484182159105937</v>
       </c>
       <c r="D6">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E6">
-        <v>0.7400107681751251</v>
+        <v>0.7546811203161875</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1204,16 +1204,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5435267857142857</v>
+        <v>0.4958333333333333</v>
       </c>
       <c r="C7">
-        <v>0.7282973442758832</v>
+        <v>0.7501791556676228</v>
       </c>
       <c r="D7">
-        <v>0.54296875</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="E7">
-        <v>0.7341943234205246</v>
+        <v>0.7412787079811096</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1221,16 +1221,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5323660714285714</v>
+        <v>0.5072916666666667</v>
       </c>
       <c r="C8">
-        <v>0.7223066219261715</v>
+        <v>0.7487317323684692</v>
       </c>
       <c r="D8">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E8">
-        <v>0.730243980884552</v>
+        <v>0.7404232621192932</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1238,16 +1238,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5368303571428571</v>
+        <v>0.4989583333333333</v>
       </c>
       <c r="C9">
-        <v>0.7185933589935303</v>
+        <v>0.7547245184580486</v>
       </c>
       <c r="D9">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E9">
-        <v>0.7299399524927139</v>
+        <v>0.7377839982509613</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1255,16 +1255,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5435267857142857</v>
+        <v>0.5177083333333333</v>
       </c>
       <c r="C10">
-        <v>0.7196304670401982</v>
+        <v>0.7508127133051554</v>
       </c>
       <c r="D10">
-        <v>0.54296875</v>
+        <v>0.5052083333333334</v>
       </c>
       <c r="E10">
-        <v>0.7252864092588425</v>
+        <v>0.7330996791521708</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1272,16 +1272,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5245535714285714</v>
+        <v>0.5447916666666667</v>
       </c>
       <c r="C11">
-        <v>0.7166946615491595</v>
+        <v>0.7311826904614767</v>
       </c>
       <c r="D11">
-        <v>0.54296875</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E11">
-        <v>0.7244364768266678</v>
+        <v>0.7362443705399832</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1289,16 +1289,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.546875</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C12">
-        <v>0.7168814071587154</v>
+        <v>0.7280039191246033</v>
       </c>
       <c r="D12">
-        <v>0.54296875</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E12">
-        <v>0.7227612286806107</v>
+        <v>0.7350746095180511</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1306,16 +1306,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5323660714285714</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="C13">
-        <v>0.7170382014342717</v>
+        <v>0.7350043177604675</v>
       </c>
       <c r="D13">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E13">
-        <v>0.7212412804365158</v>
+        <v>0.756582130988439</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1323,16 +1323,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.5323660714285714</v>
+        <v>0.509375</v>
       </c>
       <c r="C14">
-        <v>0.7157987356185913</v>
+        <v>0.7385880549748739</v>
       </c>
       <c r="D14">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E14">
-        <v>0.7201713472604752</v>
+        <v>0.7486786246299744</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1340,16 +1340,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.5379464285714286</v>
+        <v>0.5135416666666667</v>
       </c>
       <c r="C15">
-        <v>0.7154002743107932</v>
+        <v>0.7317831834157308</v>
       </c>
       <c r="D15">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E15">
-        <v>0.7191916555166245</v>
+        <v>0.7528413434823354</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1357,16 +1357,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5435267857142857</v>
+        <v>0.496875</v>
       </c>
       <c r="C16">
-        <v>0.7124066650867462</v>
+        <v>0.7405108491579692</v>
       </c>
       <c r="D16">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E16">
-        <v>0.7196387648582458</v>
+        <v>0.7440192500750223</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1374,16 +1374,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.5390625</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="C17">
-        <v>0.7102898401873452</v>
+        <v>0.7269909342130025</v>
       </c>
       <c r="D17">
-        <v>0.54296875</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E17">
-        <v>0.7184764295816422</v>
+        <v>0.7307121356328329</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1391,16 +1391,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5435267857142857</v>
+        <v>0.5114583333333333</v>
       </c>
       <c r="C18">
-        <v>0.7151241983686175</v>
+        <v>0.7287943959236145</v>
       </c>
       <c r="D18">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E18">
-        <v>0.7178189307451248</v>
+        <v>0.7277187903722128</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1408,16 +1408,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5334821428571429</v>
+        <v>0.5322916666666667</v>
       </c>
       <c r="C19">
-        <v>0.7118577361106873</v>
+        <v>0.7285622000694275</v>
       </c>
       <c r="D19">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E19">
-        <v>0.7178473621606827</v>
+        <v>0.7296323180198669</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1425,16 +1425,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5390625</v>
+        <v>0.4958333333333333</v>
       </c>
       <c r="C20">
-        <v>0.7096543993268695</v>
+        <v>0.7414008816083272</v>
       </c>
       <c r="D20">
-        <v>0.54296875</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E20">
-        <v>0.7184523642063141</v>
+        <v>0.7386084496974945</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1442,16 +1442,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.5446428571428571</v>
+        <v>0.5239583333333333</v>
       </c>
       <c r="C21">
-        <v>0.7106269129684993</v>
+        <v>0.7251156449317933</v>
       </c>
       <c r="D21">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E21">
-        <v>0.7174433022737503</v>
+        <v>0.7484180231889089</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1459,16 +1459,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.5446428571428571</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C22">
-        <v>0.7131944894790649</v>
+        <v>0.7244697769482931</v>
       </c>
       <c r="D22">
-        <v>0.54296875</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E22">
-        <v>0.7165414839982986</v>
+        <v>0.7334018250306448</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1476,16 +1476,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.5256696428571429</v>
+        <v>0.534375</v>
       </c>
       <c r="C23">
-        <v>0.7142897631440844</v>
+        <v>0.7221177339553833</v>
       </c>
       <c r="D23">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E23">
-        <v>0.7162262499332428</v>
+        <v>0.7358242273330688</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1493,16 +1493,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5390625</v>
+        <v>0.5135416666666667</v>
       </c>
       <c r="C24">
-        <v>0.7106054936136518</v>
+        <v>0.7381382584571838</v>
       </c>
       <c r="D24">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E24">
-        <v>0.7166431397199631</v>
+        <v>0.743198941151301</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1510,16 +1510,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5290178571428571</v>
+        <v>0.5072916666666667</v>
       </c>
       <c r="C25">
-        <v>0.7120069350515094</v>
+        <v>0.7248823444048563</v>
       </c>
       <c r="D25">
-        <v>0.54296875</v>
+        <v>0.5026041666666666</v>
       </c>
       <c r="E25">
-        <v>0.7158468663692474</v>
+        <v>0.7282236218452454</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1527,16 +1527,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5546875</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="C26">
-        <v>0.7090383086885724</v>
+        <v>0.7226307471593221</v>
       </c>
       <c r="D26">
-        <v>0.54296875</v>
+        <v>0.5</v>
       </c>
       <c r="E26">
-        <v>0.7158801257610321</v>
+        <v>0.7276372810204824</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1544,16 +1544,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5446428571428571</v>
+        <v>0.5354166666666667</v>
       </c>
       <c r="C27">
-        <v>0.7080963296549661</v>
+        <v>0.7180895209312439</v>
       </c>
       <c r="D27">
-        <v>0.54296875</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="E27">
-        <v>0.7156296521425247</v>
+        <v>0.7189844846725464</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1561,16 +1561,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5345982142857143</v>
+        <v>0.5354166666666667</v>
       </c>
       <c r="C28">
-        <v>0.7108101717063359</v>
+        <v>0.7226688385009765</v>
       </c>
       <c r="D28">
-        <v>0.54296875</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>0.7154268771409988</v>
+        <v>0.7278125981489817</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1578,16 +1578,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.5546875</v>
+        <v>0.53125</v>
       </c>
       <c r="C29">
-        <v>0.7086192284311567</v>
+        <v>0.7211799303690593</v>
       </c>
       <c r="D29">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E29">
-        <v>0.7176592648029327</v>
+        <v>0.7266547083854675</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1595,16 +1595,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5401785714285714</v>
+        <v>0.5479166666666667</v>
       </c>
       <c r="C30">
-        <v>0.7104186969144004</v>
+        <v>0.7196821848551432</v>
       </c>
       <c r="D30">
-        <v>0.54296875</v>
+        <v>0.4557291666666667</v>
       </c>
       <c r="E30">
-        <v>0.7150820195674896</v>
+        <v>0.7358493705590566</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1612,16 +1612,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5357142857142857</v>
+        <v>0.521875</v>
       </c>
       <c r="C31">
-        <v>0.7112796987806048</v>
+        <v>0.7270795861879985</v>
       </c>
       <c r="D31">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E31">
-        <v>0.715101882815361</v>
+        <v>0.7236616810162863</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1629,16 +1629,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5390625</v>
+        <v>0.521875</v>
       </c>
       <c r="C32">
-        <v>0.7091481813362667</v>
+        <v>0.7231133302052816</v>
       </c>
       <c r="D32">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E32">
-        <v>0.715066134929657</v>
+        <v>0.7285505831241608</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1646,16 +1646,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5301339285714286</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C33">
-        <v>0.7101681019578662</v>
+        <v>0.7305138031641643</v>
       </c>
       <c r="D33">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E33">
-        <v>0.7149715572595596</v>
+        <v>0.7471051414807638</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1663,16 +1663,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5301339285714286</v>
+        <v>0.5375</v>
       </c>
       <c r="C34">
-        <v>0.7098243151392255</v>
+        <v>0.7219629764556885</v>
       </c>
       <c r="D34">
-        <v>0.54296875</v>
+        <v>0.4609375</v>
       </c>
       <c r="E34">
-        <v>0.7155128121376038</v>
+        <v>0.7356799940268198</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1680,16 +1680,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5479910714285714</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="C35">
-        <v>0.7091469722134727</v>
+        <v>0.7163969993591308</v>
       </c>
       <c r="D35">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E35">
-        <v>0.7155701965093613</v>
+        <v>0.7468584477901459</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1697,16 +1697,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.53125</v>
+        <v>0.509375</v>
       </c>
       <c r="C36">
-        <v>0.7090166807174683</v>
+        <v>0.7260416150093079</v>
       </c>
       <c r="D36">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E36">
-        <v>0.715368315577507</v>
+        <v>0.7479411860307058</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1714,16 +1714,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.5368303571428571</v>
+        <v>0.5145833333333333</v>
       </c>
       <c r="C37">
-        <v>0.7102191192763192</v>
+        <v>0.730704132715861</v>
       </c>
       <c r="D37">
-        <v>0.54296875</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E37">
-        <v>0.7149331122636795</v>
+        <v>0.7443953355153402</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1731,16 +1731,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5379464285714286</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C38">
-        <v>0.708821931055614</v>
+        <v>0.7235353191693624</v>
       </c>
       <c r="D38">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E38">
-        <v>0.7160789221525192</v>
+        <v>0.7332979242006937</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1748,16 +1748,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.546875</v>
+        <v>0.5395833333333333</v>
       </c>
       <c r="C39">
-        <v>0.7087055487292153</v>
+        <v>0.7220621347427368</v>
       </c>
       <c r="D39">
-        <v>0.54296875</v>
+        <v>0.4635416666666667</v>
       </c>
       <c r="E39">
-        <v>0.7164539247751236</v>
+        <v>0.7384285628795624</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1765,16 +1765,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5401785714285714</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="C40">
-        <v>0.7071718190397535</v>
+        <v>0.7110157370567322</v>
       </c>
       <c r="D40">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E40">
-        <v>0.7154262810945511</v>
+        <v>0.7310362160205841</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1782,16 +1782,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5446428571428571</v>
+        <v>0.5375</v>
       </c>
       <c r="C41">
-        <v>0.708848740373339</v>
+        <v>0.7183704098065694</v>
       </c>
       <c r="D41">
-        <v>0.54296875</v>
+        <v>0.4505208333333333</v>
       </c>
       <c r="E41">
-        <v>0.7152495235204697</v>
+        <v>0.7466455201307932</v>
       </c>
     </row>
   </sheetData>
@@ -1826,16 +1826,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5234375</v>
+        <v>0.478125</v>
       </c>
       <c r="C2">
-        <v>0.8893296463148934</v>
+        <v>0.939623479048411</v>
       </c>
       <c r="D2">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E2">
-        <v>0.8167800009250641</v>
+        <v>0.8043694694836935</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5245535714285714</v>
+        <v>0.509375</v>
       </c>
       <c r="C3">
-        <v>0.7765605321952275</v>
+        <v>0.7995590607325236</v>
       </c>
       <c r="D3">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E3">
-        <v>0.7687629014253616</v>
+        <v>0.7603664298852285</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1860,16 +1860,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5368303571428571</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C4">
-        <v>0.7480229820523944</v>
+        <v>0.7752768039703369</v>
       </c>
       <c r="D4">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E4">
-        <v>0.7506925314664841</v>
+        <v>0.7455187539259592</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1877,16 +1877,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5435267857142857</v>
+        <v>0.4916666666666666</v>
       </c>
       <c r="C5">
-        <v>0.7390767804213932</v>
+        <v>0.7763124545415242</v>
       </c>
       <c r="D5">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E5">
-        <v>0.7411758899688721</v>
+        <v>0.7334982454776764</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1894,16 +1894,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5368303571428571</v>
+        <v>0.51875</v>
       </c>
       <c r="C6">
-        <v>0.7293600056852613</v>
+        <v>0.7547882199287415</v>
       </c>
       <c r="D6">
         <v>0.546875</v>
       </c>
       <c r="E6">
-        <v>0.7344342470169067</v>
+        <v>0.7289188007513682</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1911,16 +1911,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5279017857142857</v>
+        <v>0.525</v>
       </c>
       <c r="C7">
-        <v>0.7266112736293248</v>
+        <v>0.7511707623799642</v>
       </c>
       <c r="D7">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E7">
-        <v>0.7305636703968048</v>
+        <v>0.7234547436237335</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1928,16 +1928,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5256696428571429</v>
+        <v>0.4854166666666667</v>
       </c>
       <c r="C8">
-        <v>0.7245949506759644</v>
+        <v>0.7514304598172505</v>
       </c>
       <c r="D8">
-        <v>0.54296875</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E8">
-        <v>0.7311167269945145</v>
+        <v>0.7207266390323639</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1945,16 +1945,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5457589285714286</v>
+        <v>0.4760416666666666</v>
       </c>
       <c r="C9">
-        <v>0.7155521512031555</v>
+        <v>0.7531853914260864</v>
       </c>
       <c r="D9">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E9">
-        <v>0.7268331199884415</v>
+        <v>0.7182127237319946</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1962,16 +1962,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5412946428571429</v>
+        <v>0.525</v>
       </c>
       <c r="C10">
-        <v>0.7167391010693142</v>
+        <v>0.7326714158058166</v>
       </c>
       <c r="D10">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E10">
-        <v>0.7244215756654739</v>
+        <v>0.7162990470727285</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1979,16 +1979,16 @@
         <v>9</v>
       </c>
       <c r="B11">
+        <v>0.509375</v>
+      </c>
+      <c r="C11">
+        <v>0.7430218060811361</v>
+      </c>
+      <c r="D11">
         <v>0.546875</v>
       </c>
-      <c r="C11">
-        <v>0.7168237950120654</v>
-      </c>
-      <c r="D11">
-        <v>0.54296875</v>
-      </c>
       <c r="E11">
-        <v>0.7231090664863586</v>
+        <v>0.716057668129603</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1996,16 +1996,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.5267857142857143</v>
+        <v>0.534375</v>
       </c>
       <c r="C12">
-        <v>0.7166536450386047</v>
+        <v>0.7366705536842346</v>
       </c>
       <c r="D12">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E12">
-        <v>0.7220065891742706</v>
+        <v>0.714616060256958</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2013,16 +2013,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5357142857142857</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="C13">
-        <v>0.7127790536199298</v>
+        <v>0.744925053914388</v>
       </c>
       <c r="D13">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E13">
-        <v>0.7261186987161636</v>
+        <v>0.7146251598993937</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2030,16 +2030,16 @@
         <v>12</v>
       </c>
       <c r="B14">
+        <v>0.503125</v>
+      </c>
+      <c r="C14">
+        <v>0.7446587125460307</v>
+      </c>
+      <c r="D14">
         <v>0.546875</v>
       </c>
-      <c r="C14">
-        <v>0.7139211084161486</v>
-      </c>
-      <c r="D14">
-        <v>0.54296875</v>
-      </c>
       <c r="E14">
-        <v>0.7255668938159943</v>
+        <v>0.7139193117618561</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2047,16 +2047,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.5390625</v>
+        <v>0.5125</v>
       </c>
       <c r="C15">
-        <v>0.7128611334732601</v>
+        <v>0.7323893825213115</v>
       </c>
       <c r="D15">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E15">
-        <v>0.720519095659256</v>
+        <v>0.7136787672837576</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2064,16 +2064,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5334821428571429</v>
+        <v>0.5104166666666666</v>
       </c>
       <c r="C16">
-        <v>0.7124227200235639</v>
+        <v>0.7314379135767619</v>
       </c>
       <c r="D16">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E16">
-        <v>0.7226031124591827</v>
+        <v>0.7129860619703928</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2081,16 +2081,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.5457589285714286</v>
+        <v>0.515625</v>
       </c>
       <c r="C17">
-        <v>0.7117682482515063</v>
+        <v>0.7330052693684895</v>
       </c>
       <c r="D17">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E17">
-        <v>0.721435159444809</v>
+        <v>0.7124528388182322</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2098,16 +2098,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5424107142857143</v>
+        <v>0.5125</v>
       </c>
       <c r="C18">
-        <v>0.7095510278429303</v>
+        <v>0.7323892951011658</v>
       </c>
       <c r="D18">
-        <v>0.54296875</v>
+        <v>0.5546875</v>
       </c>
       <c r="E18">
-        <v>0.7198021858930588</v>
+        <v>0.7139073411623637</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2115,16 +2115,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5524553571428571</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C19">
-        <v>0.7084047794342041</v>
+        <v>0.7282405535380045</v>
       </c>
       <c r="D19">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E19">
-        <v>0.7191798686981201</v>
+        <v>0.7122912307580312</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2132,16 +2132,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5513392857142857</v>
+        <v>0.5177083333333333</v>
       </c>
       <c r="C20">
-        <v>0.7103725458894458</v>
+        <v>0.7335966904958089</v>
       </c>
       <c r="D20">
-        <v>0.54296875</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E20">
-        <v>0.7209882885217667</v>
+        <v>0.7126410106817881</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2149,16 +2149,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.5535714285714286</v>
+        <v>0.51875</v>
       </c>
       <c r="C21">
-        <v>0.7072511145046779</v>
+        <v>0.7282183289527893</v>
       </c>
       <c r="D21">
-        <v>0.54296875</v>
+        <v>0.5546875</v>
       </c>
       <c r="E21">
-        <v>0.722056657075882</v>
+        <v>0.7134569485982259</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2166,16 +2166,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.5625</v>
+        <v>0.5145833333333333</v>
       </c>
       <c r="C22">
-        <v>0.7083673817770821</v>
+        <v>0.7290706793467204</v>
       </c>
       <c r="D22">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E22">
-        <v>0.7294639199972153</v>
+        <v>0.7136586705843607</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2183,16 +2183,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.5345982142857143</v>
+        <v>0.509375</v>
       </c>
       <c r="C23">
-        <v>0.710090662751879</v>
+        <v>0.7297090967496236</v>
       </c>
       <c r="D23">
-        <v>0.54296875</v>
+        <v>0.4739583333333333</v>
       </c>
       <c r="E23">
-        <v>0.7241074442863464</v>
+        <v>0.7154048879941305</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2200,16 +2200,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5390625</v>
+        <v>0.5375</v>
       </c>
       <c r="C24">
-        <v>0.7100329101085663</v>
+        <v>0.724796458085378</v>
       </c>
       <c r="D24">
-        <v>0.54296875</v>
+        <v>0.453125</v>
       </c>
       <c r="E24">
-        <v>0.7230397760868073</v>
+        <v>0.7168476382891337</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2217,16 +2217,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5301339285714286</v>
+        <v>0.4989583333333333</v>
       </c>
       <c r="C25">
-        <v>0.7117443297590528</v>
+        <v>0.7271899819374085</v>
       </c>
       <c r="D25">
-        <v>0.54296875</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E25">
-        <v>0.7187861949205399</v>
+        <v>0.7121692796548208</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2234,16 +2234,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5524553571428571</v>
+        <v>0.5322916666666667</v>
       </c>
       <c r="C26">
-        <v>0.7061267026833126</v>
+        <v>0.7223262151082357</v>
       </c>
       <c r="D26">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E26">
-        <v>0.7282138764858246</v>
+        <v>0.7152105371157328</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2251,16 +2251,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5424107142857143</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="C27">
-        <v>0.7110821349280221</v>
+        <v>0.7239583293596904</v>
       </c>
       <c r="D27">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E27">
-        <v>0.7235143929719925</v>
+        <v>0.7111914753913879</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2268,16 +2268,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5502232142857143</v>
+        <v>0.521875</v>
       </c>
       <c r="C28">
-        <v>0.7055606331144061</v>
+        <v>0.7224124630292257</v>
       </c>
       <c r="D28">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E28">
-        <v>0.7182310074567795</v>
+        <v>0.7111704647541046</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2285,16 +2285,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.5223214285714286</v>
+        <v>0.4989583333333333</v>
       </c>
       <c r="C29">
-        <v>0.7071168507848468</v>
+        <v>0.7327961246172587</v>
       </c>
       <c r="D29">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E29">
-        <v>0.7211575359106064</v>
+        <v>0.7134848237037659</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2302,16 +2302,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5368303571428571</v>
+        <v>0.521875</v>
       </c>
       <c r="C30">
-        <v>0.7082335225173405</v>
+        <v>0.7260449608167012</v>
       </c>
       <c r="D30">
-        <v>0.54296875</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E30">
-        <v>0.721114918589592</v>
+        <v>0.7118937373161316</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2319,16 +2319,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5435267857142857</v>
+        <v>0.5135416666666667</v>
       </c>
       <c r="C31">
-        <v>0.7080533972808293</v>
+        <v>0.7256051460901897</v>
       </c>
       <c r="D31">
-        <v>0.54296875</v>
+        <v>0.546875</v>
       </c>
       <c r="E31">
-        <v>0.7233351320028305</v>
+        <v>0.7112407584985098</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2336,16 +2336,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5379464285714286</v>
+        <v>0.540625</v>
       </c>
       <c r="C32">
-        <v>0.7052146920136043</v>
+        <v>0.7194580554962158</v>
       </c>
       <c r="D32">
-        <v>0.54296875</v>
+        <v>0.5286458333333334</v>
       </c>
       <c r="E32">
-        <v>0.7274062037467957</v>
+        <v>0.7128148972988129</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2353,16 +2353,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5390625</v>
+        <v>0.553125</v>
       </c>
       <c r="C33">
-        <v>0.7097613130296979</v>
+        <v>0.7210059881210327</v>
       </c>
       <c r="D33">
-        <v>0.54296875</v>
+        <v>0.5286458333333334</v>
       </c>
       <c r="E33">
-        <v>0.7213306874036789</v>
+        <v>0.7125814259052277</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2370,16 +2370,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5379464285714286</v>
+        <v>0.5145833333333333</v>
       </c>
       <c r="C34">
-        <v>0.7112515313284737</v>
+        <v>0.7251500686009725</v>
       </c>
       <c r="D34">
-        <v>0.54296875</v>
+        <v>0.46875</v>
       </c>
       <c r="E34">
-        <v>0.7207122445106506</v>
+        <v>0.7137924333413442</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2387,16 +2387,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5491071428571429</v>
+        <v>0.53125</v>
       </c>
       <c r="C35">
-        <v>0.7040591027055468</v>
+        <v>0.7180702368418376</v>
       </c>
       <c r="D35">
-        <v>0.54296875</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E35">
-        <v>0.7192193269729614</v>
+        <v>0.7135062913099924</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2404,16 +2404,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.5513392857142857</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="C36">
-        <v>0.7081409990787506</v>
+        <v>0.7155745188395183</v>
       </c>
       <c r="D36">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E36">
-        <v>0.7162598669528961</v>
+        <v>0.7123572130997976</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2421,16 +2421,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.5580357142857143</v>
+        <v>0.5458333333333333</v>
       </c>
       <c r="C37">
-        <v>0.7084838492529733</v>
+        <v>0.7124794363975525</v>
       </c>
       <c r="D37">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E37">
-        <v>0.7193709760904312</v>
+        <v>0.7125787238279978</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2438,16 +2438,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5368303571428571</v>
+        <v>0.540625</v>
       </c>
       <c r="C38">
-        <v>0.7048210075923375</v>
+        <v>0.7239739457766216</v>
       </c>
       <c r="D38">
-        <v>0.54296875</v>
+        <v>0.4713541666666667</v>
       </c>
       <c r="E38">
-        <v>0.7317080050706863</v>
+        <v>0.7165550192197164</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2455,16 +2455,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.5334821428571429</v>
+        <v>0.50625</v>
       </c>
       <c r="C39">
-        <v>0.7086155968053001</v>
+        <v>0.7322618087132772</v>
       </c>
       <c r="D39">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E39">
-        <v>0.7316967844963074</v>
+        <v>0.7171250879764557</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2472,16 +2472,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5491071428571429</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C40">
-        <v>0.7054412024361747</v>
+        <v>0.7172965010007223</v>
       </c>
       <c r="D40">
-        <v>0.54296875</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E40">
-        <v>0.7303701341152191</v>
+        <v>0.7147137820720673</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2489,16 +2489,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5368303571428571</v>
+        <v>0.5322916666666667</v>
       </c>
       <c r="C41">
-        <v>0.7065192035266331</v>
+        <v>0.7190415700276692</v>
       </c>
       <c r="D41">
-        <v>0.54296875</v>
+        <v>0.4713541666666667</v>
       </c>
       <c r="E41">
-        <v>0.7261070758104324</v>
+        <v>0.7160590291023254</v>
       </c>
     </row>
   </sheetData>
@@ -2533,16 +2533,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5223214285714286</v>
+        <v>0.48125</v>
       </c>
       <c r="C2">
-        <v>0.9079947301319667</v>
+        <v>0.9392464995384217</v>
       </c>
       <c r="D2">
-        <v>0.54296875</v>
+        <v>0.5052083333333334</v>
       </c>
       <c r="E2">
-        <v>0.8337315022945404</v>
+        <v>0.8107729355494181</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2550,16 +2550,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5424107142857143</v>
+        <v>0.534375</v>
       </c>
       <c r="C3">
-        <v>0.7804538309574127</v>
+        <v>0.7971000035603841</v>
       </c>
       <c r="D3">
-        <v>0.54296875</v>
+        <v>0.5130208333333334</v>
       </c>
       <c r="E3">
-        <v>0.7800000607967377</v>
+        <v>0.7679737905661265</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2567,16 +2567,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5435267857142857</v>
+        <v>0.5041666666666667</v>
       </c>
       <c r="C4">
-        <v>0.7516790798732212</v>
+        <v>0.7814840237299602</v>
       </c>
       <c r="D4">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E4">
-        <v>0.7561240941286087</v>
+        <v>0.7538671890894572</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2584,16 +2584,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5479910714285714</v>
+        <v>0.5072916666666667</v>
       </c>
       <c r="C5">
-        <v>0.7369376165526254</v>
+        <v>0.7626415530840556</v>
       </c>
       <c r="D5">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E5">
-        <v>0.7439927607774734</v>
+        <v>0.7464878161748251</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2601,16 +2601,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5401785714285714</v>
+        <v>0.4927083333333334</v>
       </c>
       <c r="C6">
-        <v>0.7301058854375567</v>
+        <v>0.7543750325838725</v>
       </c>
       <c r="D6">
-        <v>0.54296875</v>
+        <v>0.4765625</v>
       </c>
       <c r="E6">
-        <v>0.7382681965827942</v>
+        <v>0.7405242025852203</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2618,16 +2618,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5591517857142857</v>
+        <v>0.5322916666666667</v>
       </c>
       <c r="C7">
-        <v>0.7240395758833204</v>
+        <v>0.7399768710136414</v>
       </c>
       <c r="D7">
-        <v>0.54296875</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E7">
-        <v>0.7335408329963684</v>
+        <v>0.7399784028530121</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2635,16 +2635,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5424107142857143</v>
+        <v>0.5104166666666666</v>
       </c>
       <c r="C8">
-        <v>0.7222800212247031</v>
+        <v>0.7440829992294311</v>
       </c>
       <c r="D8">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E8">
-        <v>0.7284052670001984</v>
+        <v>0.7357618908087412</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2652,16 +2652,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5401785714285714</v>
+        <v>0.5114583333333333</v>
       </c>
       <c r="C9">
-        <v>0.7186290068285806</v>
+        <v>0.7558284719785054</v>
       </c>
       <c r="D9">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E9">
-        <v>0.7254321724176407</v>
+        <v>0.7339389622211456</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2669,16 +2669,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5446428571428571</v>
+        <v>0.5270833333333333</v>
       </c>
       <c r="C10">
-        <v>0.7169592295374189</v>
+        <v>0.7399688204129536</v>
       </c>
       <c r="D10">
-        <v>0.54296875</v>
+        <v>0.4973958333333333</v>
       </c>
       <c r="E10">
-        <v>0.7237649112939835</v>
+        <v>0.7403686046600342</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2686,16 +2686,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5446428571428571</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C11">
-        <v>0.7171129924910409</v>
+        <v>0.7307880640029907</v>
       </c>
       <c r="D11">
-        <v>0.54296875</v>
+        <v>0.5026041666666666</v>
       </c>
       <c r="E11">
-        <v>0.7221376448869705</v>
+        <v>0.7384790182113647</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2703,16 +2703,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.5390625</v>
+        <v>0.525</v>
       </c>
       <c r="C12">
-        <v>0.7153734607355935</v>
+        <v>0.7291636347770691</v>
       </c>
       <c r="D12">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E12">
-        <v>0.7213875502347946</v>
+        <v>0.7311339577039083</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2720,16 +2720,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5513392857142857</v>
+        <v>0.5239583333333333</v>
       </c>
       <c r="C13">
-        <v>0.7144227411065783</v>
+        <v>0.7377597729365031</v>
       </c>
       <c r="D13">
-        <v>0.54296875</v>
+        <v>0.4973958333333333</v>
       </c>
       <c r="E13">
-        <v>0.7203604280948639</v>
+        <v>0.7372537056605021</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2737,16 +2737,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.5379464285714286</v>
+        <v>0.546875</v>
       </c>
       <c r="C14">
-        <v>0.7131389038903373</v>
+        <v>0.7238503615061442</v>
       </c>
       <c r="D14">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E14">
-        <v>0.7200635522603989</v>
+        <v>0.7351841231187185</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2754,16 +2754,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.5457589285714286</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C15">
-        <v>0.712811814887183</v>
+        <v>0.7270131508509318</v>
       </c>
       <c r="D15">
-        <v>0.54296875</v>
+        <v>0.4713541666666667</v>
       </c>
       <c r="E15">
-        <v>0.7185626327991486</v>
+        <v>0.7436189452807108</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2771,16 +2771,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5491071428571429</v>
+        <v>0.4822916666666667</v>
       </c>
       <c r="C16">
-        <v>0.7126293395246778</v>
+        <v>0.7396128416061402</v>
       </c>
       <c r="D16">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E16">
-        <v>0.7186215072870255</v>
+        <v>0.7328620851039886</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2788,16 +2788,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.5390625</v>
+        <v>0.5447916666666667</v>
       </c>
       <c r="C17">
-        <v>0.7122931139809745</v>
+        <v>0.7188659111658732</v>
       </c>
       <c r="D17">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E17">
-        <v>0.7187150567770004</v>
+        <v>0.7313444018363953</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2805,16 +2805,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5513392857142857</v>
+        <v>0.50625</v>
       </c>
       <c r="C18">
-        <v>0.7095135280064174</v>
+        <v>0.7388206084569295</v>
       </c>
       <c r="D18">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E18">
-        <v>0.7227903753519058</v>
+        <v>0.7329505582650503</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2822,16 +2822,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.546875</v>
+        <v>0.54375</v>
       </c>
       <c r="C19">
-        <v>0.7104464088167463</v>
+        <v>0.7299658377965291</v>
       </c>
       <c r="D19">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E19">
-        <v>0.7179144620895386</v>
+        <v>0.7374417384465536</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2839,16 +2839,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5412946428571429</v>
+        <v>0.5447916666666667</v>
       </c>
       <c r="C20">
-        <v>0.7088626580578941</v>
+        <v>0.7197834054629008</v>
       </c>
       <c r="D20">
-        <v>0.54296875</v>
+        <v>0.484375</v>
       </c>
       <c r="E20">
-        <v>0.7176237255334854</v>
+        <v>0.7356970310211182</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2856,16 +2856,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.546875</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="C21">
-        <v>0.7092606212411608</v>
+        <v>0.738375727335612</v>
       </c>
       <c r="D21">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E21">
-        <v>0.7172428965568542</v>
+        <v>0.7351403832435608</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2873,16 +2873,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.546875</v>
+        <v>0.534375</v>
       </c>
       <c r="C22">
-        <v>0.7091349405901772</v>
+        <v>0.7254484931627909</v>
       </c>
       <c r="D22">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E22">
-        <v>0.7169658839702606</v>
+        <v>0.7295015553633372</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2890,16 +2890,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.5602678571428571</v>
+        <v>0.53125</v>
       </c>
       <c r="C23">
-        <v>0.7095634852136884</v>
+        <v>0.7212026079495748</v>
       </c>
       <c r="D23">
-        <v>0.54296875</v>
+        <v>0.4973958333333333</v>
       </c>
       <c r="E23">
-        <v>0.7168878763914108</v>
+        <v>0.7305282354354858</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2907,16 +2907,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.546875</v>
+        <v>0.5302083333333333</v>
       </c>
       <c r="C24">
-        <v>0.7097053016935077</v>
+        <v>0.7280175964037577</v>
       </c>
       <c r="D24">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E24">
-        <v>0.7165473401546478</v>
+        <v>0.746606687704722</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2924,16 +2924,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5368303571428571</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="C25">
-        <v>0.7115992222513471</v>
+        <v>0.7221794764200846</v>
       </c>
       <c r="D25">
-        <v>0.54296875</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>0.7163975685834885</v>
+        <v>0.7422564923763275</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2941,16 +2941,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5390625</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="C26">
-        <v>0.7097477103982653</v>
+        <v>0.7256843725840251</v>
       </c>
       <c r="D26">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E26">
-        <v>0.7168874442577362</v>
+        <v>0.7356749176979065</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2958,16 +2958,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5479910714285714</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="C27">
-        <v>0.7099268479006631</v>
+        <v>0.716357700030009</v>
       </c>
       <c r="D27">
-        <v>0.54296875</v>
+        <v>0.4947916666666667</v>
       </c>
       <c r="E27">
-        <v>0.7160476744174957</v>
+        <v>0.7473896046479543</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2975,16 +2975,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5502232142857143</v>
+        <v>0.5375</v>
       </c>
       <c r="C28">
-        <v>0.7086701222828456</v>
+        <v>0.7273816347122193</v>
       </c>
       <c r="D28">
-        <v>0.54296875</v>
+        <v>0.4973958333333333</v>
       </c>
       <c r="E28">
-        <v>0.7160927057266235</v>
+        <v>0.7434841593106588</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2992,16 +2992,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.546875</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C29">
-        <v>0.7077255717345646</v>
+        <v>0.7236804962158203</v>
       </c>
       <c r="D29">
-        <v>0.54296875</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
-        <v>0.7157799154520035</v>
+        <v>0.7488565345605215</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3009,16 +3009,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5412946428571429</v>
+        <v>0.5447916666666667</v>
       </c>
       <c r="C30">
-        <v>0.7077702837330955</v>
+        <v>0.7189718166987101</v>
       </c>
       <c r="D30">
-        <v>0.52734375</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E30">
-        <v>0.7157999724149704</v>
+        <v>0.7394570012887319</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3026,16 +3026,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5535714285714286</v>
+        <v>0.5260416666666666</v>
       </c>
       <c r="C31">
-        <v>0.7089881982122149</v>
+        <v>0.7198820034662883</v>
       </c>
       <c r="D31">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E31">
-        <v>0.7168231606483459</v>
+        <v>0.7471535205841064</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3043,16 +3043,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5357142857142857</v>
+        <v>0.5302083333333333</v>
       </c>
       <c r="C32">
-        <v>0.709612386567252</v>
+        <v>0.7206239223480224</v>
       </c>
       <c r="D32">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E32">
-        <v>0.7154567539691925</v>
+        <v>0.7406357129414877</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3060,16 +3060,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5446428571428571</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="C33">
-        <v>0.7088314848286765</v>
+        <v>0.7272732496261597</v>
       </c>
       <c r="D33">
-        <v>0.54296875</v>
+        <v>0.5026041666666666</v>
       </c>
       <c r="E33">
-        <v>0.7155001759529114</v>
+        <v>0.7474037806193033</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3077,16 +3077,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5479910714285714</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="C34">
-        <v>0.7079586386680603</v>
+        <v>0.7231303453445435</v>
       </c>
       <c r="D34">
-        <v>0.54296875</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="E34">
-        <v>0.7166966050863266</v>
+        <v>0.742595911026001</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3094,16 +3094,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5502232142857143</v>
+        <v>0.5177083333333333</v>
       </c>
       <c r="C35">
-        <v>0.7087322856698718</v>
+        <v>0.724616285165151</v>
       </c>
       <c r="D35">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E35">
-        <v>0.7156877368688583</v>
+        <v>0.7441300551096598</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3111,16 +3111,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.546875</v>
+        <v>0.521875</v>
       </c>
       <c r="C36">
-        <v>0.708639498267855</v>
+        <v>0.7265557169914245</v>
       </c>
       <c r="D36">
-        <v>0.54296875</v>
+        <v>0.4869791666666667</v>
       </c>
       <c r="E36">
-        <v>0.7148883193731308</v>
+        <v>0.7451314032077789</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3128,16 +3128,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.546875</v>
+        <v>0.51875</v>
       </c>
       <c r="C37">
-        <v>0.7090486586093903</v>
+        <v>0.727496325969696</v>
       </c>
       <c r="D37">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E37">
-        <v>0.7153318971395493</v>
+        <v>0.7660445173581442</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3145,16 +3145,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5390625</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C38">
-        <v>0.7086296592439923</v>
+        <v>0.7238811651865641</v>
       </c>
       <c r="D38">
-        <v>0.54296875</v>
+        <v>0.5026041666666666</v>
       </c>
       <c r="E38">
-        <v>0.7159083932638168</v>
+        <v>0.748742014169693</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3162,16 +3162,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.5390625</v>
+        <v>0.55625</v>
       </c>
       <c r="C39">
-        <v>0.7076756656169891</v>
+        <v>0.714823059240977</v>
       </c>
       <c r="D39">
-        <v>0.54296875</v>
+        <v>0.5</v>
       </c>
       <c r="E39">
-        <v>0.7152013629674911</v>
+        <v>0.7494803071022034</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3179,16 +3179,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5435267857142857</v>
+        <v>0.5510416666666667</v>
       </c>
       <c r="C40">
-        <v>0.7065372509615762</v>
+        <v>0.7174777785936991</v>
       </c>
       <c r="D40">
-        <v>0.54296875</v>
+        <v>0.4817708333333333</v>
       </c>
       <c r="E40">
-        <v>0.7152293026447296</v>
+        <v>0.7613863050937653</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3196,16 +3196,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5345982142857143</v>
+        <v>0.51875</v>
       </c>
       <c r="C41">
-        <v>0.7090404672282082</v>
+        <v>0.7173761288324992</v>
       </c>
       <c r="D41">
-        <v>0.54296875</v>
+        <v>0.4921875</v>
       </c>
       <c r="E41">
-        <v>0.7153079658746719</v>
+        <v>0.7543487052122752</v>
       </c>
     </row>
   </sheetData>
@@ -3240,16 +3240,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3627232142857143</v>
+        <v>0.5104166666666666</v>
       </c>
       <c r="C2">
-        <v>1.019002688782556</v>
+        <v>0.8801116108894348</v>
       </c>
       <c r="D2">
-        <v>0.44140625</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E2">
-        <v>0.8810623437166214</v>
+        <v>0.808460126320521</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3257,16 +3257,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5245535714285714</v>
+        <v>0.5197916666666667</v>
       </c>
       <c r="C3">
-        <v>0.8123282279287066</v>
+        <v>0.7868059714635213</v>
       </c>
       <c r="D3">
-        <v>0.515625</v>
+        <v>0.5546875</v>
       </c>
       <c r="E3">
-        <v>0.7935867756605148</v>
+        <v>0.765269011259079</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3274,16 +3274,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5446428571428571</v>
+        <v>0.5010416666666667</v>
       </c>
       <c r="C4">
-        <v>0.7677077523299626</v>
+        <v>0.7764079411824544</v>
       </c>
       <c r="D4">
-        <v>0.515625</v>
+        <v>0.5546875</v>
       </c>
       <c r="E4">
-        <v>0.7623893022537231</v>
+        <v>0.7505585551261902</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3291,16 +3291,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5401785714285714</v>
+        <v>0.5052083333333334</v>
       </c>
       <c r="C5">
-        <v>0.7492337312017169</v>
+        <v>0.7658898830413818</v>
       </c>
       <c r="D5">
-        <v>0.546875</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E5">
-        <v>0.7485281080007553</v>
+        <v>0.736033707857132</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3308,16 +3308,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5245535714285714</v>
+        <v>0.503125</v>
       </c>
       <c r="C6">
-        <v>0.7388902604579926</v>
+        <v>0.7516351938247681</v>
       </c>
       <c r="D6">
-        <v>0.546875</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E6">
-        <v>0.73737633228302</v>
+        <v>0.7282814184824625</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3325,16 +3325,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5424107142857143</v>
+        <v>0.521875</v>
       </c>
       <c r="C7">
-        <v>0.732286376612527</v>
+        <v>0.7505777676900228</v>
       </c>
       <c r="D7">
-        <v>0.546875</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E7">
-        <v>0.7342256009578705</v>
+        <v>0.72419673204422</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3342,16 +3342,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5357142857142857</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="C8">
-        <v>0.7259568657193866</v>
+        <v>0.7332811633745829</v>
       </c>
       <c r="D8">
-        <v>0.5390625</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E8">
-        <v>0.7267135828733444</v>
+        <v>0.7239724695682526</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3359,16 +3359,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5212053571428571</v>
+        <v>0.534375</v>
       </c>
       <c r="C9">
-        <v>0.7280965106827872</v>
+        <v>0.737199068069458</v>
       </c>
       <c r="D9">
-        <v>0.55078125</v>
+        <v>0.546875</v>
       </c>
       <c r="E9">
-        <v>0.7242717295885086</v>
+        <v>0.7197111348311106</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3376,16 +3376,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5345982142857143</v>
+        <v>0.5125</v>
       </c>
       <c r="C10">
-        <v>0.7212935473237719</v>
+        <v>0.7424657543500265</v>
       </c>
       <c r="D10">
-        <v>0.546875</v>
+        <v>0.5546875</v>
       </c>
       <c r="E10">
-        <v>0.721874862909317</v>
+        <v>0.717549999554952</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3393,16 +3393,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5446428571428571</v>
+        <v>0.5135416666666667</v>
       </c>
       <c r="C11">
-        <v>0.7175052762031555</v>
+        <v>0.738296643892924</v>
       </c>
       <c r="D11">
-        <v>0.5390625</v>
+        <v>0.5546875</v>
       </c>
       <c r="E11">
-        <v>0.7196473181247711</v>
+        <v>0.7198490003744761</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3410,16 +3410,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.5446428571428571</v>
+        <v>0.503125</v>
       </c>
       <c r="C12">
-        <v>0.7147157617977687</v>
+        <v>0.7431042949358623</v>
       </c>
       <c r="D12">
-        <v>0.546875</v>
+        <v>0.5546875</v>
       </c>
       <c r="E12">
-        <v>0.7183962464332581</v>
+        <v>0.7192584971586863</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3427,16 +3427,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5345982142857143</v>
+        <v>0.528125</v>
       </c>
       <c r="C13">
-        <v>0.7175654896668026</v>
+        <v>0.7389147758483887</v>
       </c>
       <c r="D13">
-        <v>0.54296875</v>
+        <v>0.5546875</v>
       </c>
       <c r="E13">
-        <v>0.7170325368642807</v>
+        <v>0.7161101301511129</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3444,16 +3444,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.5301339285714286</v>
+        <v>0.525</v>
       </c>
       <c r="C14">
-        <v>0.7161168200629098</v>
+        <v>0.734835946559906</v>
       </c>
       <c r="D14">
-        <v>0.54296875</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E14">
-        <v>0.7171785682439804</v>
+        <v>0.7133438487847646</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3461,16 +3461,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.5424107142857143</v>
+        <v>0.5041666666666667</v>
       </c>
       <c r="C15">
-        <v>0.7141528683049339</v>
+        <v>0.7403741757074992</v>
       </c>
       <c r="D15">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E15">
-        <v>0.7179014533758163</v>
+        <v>0.7155467470486959</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3478,16 +3478,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5435267857142857</v>
+        <v>0.515625</v>
       </c>
       <c r="C16">
-        <v>0.7147024742194584</v>
+        <v>0.7393929719924927</v>
       </c>
       <c r="D16">
-        <v>0.53515625</v>
+        <v>0.5546875</v>
       </c>
       <c r="E16">
-        <v>0.7187118530273438</v>
+        <v>0.7150304516156515</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3495,16 +3495,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.5267857142857143</v>
+        <v>0.55</v>
       </c>
       <c r="C17">
-        <v>0.7158112483365195</v>
+        <v>0.7281607190767924</v>
       </c>
       <c r="D17">
-        <v>0.546875</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E17">
-        <v>0.7145532220602036</v>
+        <v>0.7130318880081177</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3512,16 +3512,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5279017857142857</v>
+        <v>0.5114583333333333</v>
       </c>
       <c r="C18">
-        <v>0.7139852515288762</v>
+        <v>0.742164146900177</v>
       </c>
       <c r="D18">
-        <v>0.546875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E18">
-        <v>0.7143580913543701</v>
+        <v>0.7171603441238403</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3529,16 +3529,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5412946428571429</v>
+        <v>0.5010416666666667</v>
       </c>
       <c r="C19">
-        <v>0.7126823025090354</v>
+        <v>0.7385069370269776</v>
       </c>
       <c r="D19">
-        <v>0.54296875</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E19">
-        <v>0.7155022174119949</v>
+        <v>0.7123487492402395</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3546,16 +3546,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5401785714285714</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="C20">
-        <v>0.7118510859353202</v>
+        <v>0.724254580338796</v>
       </c>
       <c r="D20">
-        <v>0.55078125</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E20">
-        <v>0.7142353057861328</v>
+        <v>0.7145053247610728</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3563,16 +3563,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.5502232142857143</v>
+        <v>0.540625</v>
       </c>
       <c r="C21">
-        <v>0.7105039826461247</v>
+        <v>0.7255555033683777</v>
       </c>
       <c r="D21">
-        <v>0.54296875</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="E21">
-        <v>0.7130467891693115</v>
+        <v>0.7090408504009247</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3580,16 +3580,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.5390625</v>
+        <v>0.5041666666666667</v>
       </c>
       <c r="C22">
-        <v>0.7110883593559265</v>
+        <v>0.7287726481755574</v>
       </c>
       <c r="D22">
-        <v>0.53515625</v>
+        <v>0.5625</v>
       </c>
       <c r="E22">
-        <v>0.7150744944810867</v>
+        <v>0.7086594700813293</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3597,16 +3597,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.5479910714285714</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="C23">
-        <v>0.7118934776101794</v>
+        <v>0.7278884569803874</v>
       </c>
       <c r="D23">
-        <v>0.53515625</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E23">
-        <v>0.7142155766487122</v>
+        <v>0.7083328266938528</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3614,16 +3614,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5345982142857143</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="C24">
-        <v>0.7133090921810695</v>
+        <v>0.7211783369382222</v>
       </c>
       <c r="D24">
-        <v>0.54296875</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E24">
-        <v>0.7135429084300995</v>
+        <v>0.7071077227592468</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3631,16 +3631,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5435267857142857</v>
+        <v>0.528125</v>
       </c>
       <c r="C25">
-        <v>0.7089687756129673</v>
+        <v>0.7245865424474081</v>
       </c>
       <c r="D25">
-        <v>0.546875</v>
+        <v>0.5625</v>
       </c>
       <c r="E25">
-        <v>0.7124052196741104</v>
+        <v>0.7076245844364166</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3648,16 +3648,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5446428571428571</v>
+        <v>0.5020833333333333</v>
       </c>
       <c r="C26">
-        <v>0.7099815734795162</v>
+        <v>0.7388180216153463</v>
       </c>
       <c r="D26">
-        <v>0.53125</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E26">
-        <v>0.7145958840847015</v>
+        <v>0.7074017226696014</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3665,16 +3665,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5491071428571429</v>
+        <v>0.5270833333333333</v>
       </c>
       <c r="C27">
-        <v>0.7087488685335431</v>
+        <v>0.7254854321479798</v>
       </c>
       <c r="D27">
-        <v>0.55078125</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E27">
-        <v>0.7108182311058044</v>
+        <v>0.7066708405812582</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3682,16 +3682,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5457589285714286</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C28">
-        <v>0.7087824429784503</v>
+        <v>0.7278677821159363</v>
       </c>
       <c r="D28">
-        <v>0.53125</v>
+        <v>0.5494791666666666</v>
       </c>
       <c r="E28">
-        <v>0.7146171629428864</v>
+        <v>0.7077217400074005</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3699,16 +3699,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.5457589285714286</v>
+        <v>0.528125</v>
       </c>
       <c r="C29">
-        <v>0.7097659068448203</v>
+        <v>0.7255060354868571</v>
       </c>
       <c r="D29">
-        <v>0.53515625</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E29">
-        <v>0.7138227969408035</v>
+        <v>0.7061728139718374</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3716,16 +3716,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5279017857142857</v>
+        <v>0.5385416666666667</v>
       </c>
       <c r="C30">
-        <v>0.7084575806345258</v>
+        <v>0.7300836165746053</v>
       </c>
       <c r="D30">
-        <v>0.546875</v>
+        <v>0.5651041666666666</v>
       </c>
       <c r="E30">
-        <v>0.7104626297950745</v>
+        <v>0.7070940832297007</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3733,16 +3733,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5524553571428571</v>
+        <v>0.5239583333333333</v>
       </c>
       <c r="C31">
-        <v>0.709543547460011</v>
+        <v>0.7266589721043905</v>
       </c>
       <c r="D31">
-        <v>0.55078125</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E31">
-        <v>0.7102842628955841</v>
+        <v>0.7069489459196726</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3750,16 +3750,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5479910714285714</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="C32">
-        <v>0.708759069442749</v>
+        <v>0.7150932828585307</v>
       </c>
       <c r="D32">
-        <v>0.546875</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E32">
-        <v>0.7102389931678772</v>
+        <v>0.7071612775325775</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3767,16 +3767,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5491071428571429</v>
+        <v>0.521875</v>
       </c>
       <c r="C33">
-        <v>0.7078238810811724</v>
+        <v>0.7208698471387227</v>
       </c>
       <c r="D33">
-        <v>0.546875</v>
+        <v>0.5677083333333334</v>
       </c>
       <c r="E33">
-        <v>0.7103346586227417</v>
+        <v>0.7069952388604482</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3784,16 +3784,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5424107142857143</v>
+        <v>0.5145833333333333</v>
       </c>
       <c r="C34">
-        <v>0.7096880035740989</v>
+        <v>0.7255913098653157</v>
       </c>
       <c r="D34">
-        <v>0.5390625</v>
+        <v>0.5572916666666666</v>
       </c>
       <c r="E34">
-        <v>0.7114741504192352</v>
+        <v>0.7065859138965607</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3801,16 +3801,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5558035714285714</v>
+        <v>0.5364583333333334</v>
       </c>
       <c r="C35">
-        <v>0.7107510609286172</v>
+        <v>0.7275947690010071</v>
       </c>
       <c r="D35">
-        <v>0.53125</v>
+        <v>0.5546875</v>
       </c>
       <c r="E35">
-        <v>0.7115237414836884</v>
+        <v>0.708234558502833</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3818,16 +3818,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.5513392857142857</v>
+        <v>0.5375</v>
       </c>
       <c r="C36">
-        <v>0.7066218427249363</v>
+        <v>0.7190467635790507</v>
       </c>
       <c r="D36">
-        <v>0.53125</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="E36">
-        <v>0.7134635895490646</v>
+        <v>0.7070229152838389</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3835,16 +3835,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.5591517857142857</v>
+        <v>0.5354166666666667</v>
       </c>
       <c r="C37">
-        <v>0.7060469346387046</v>
+        <v>0.7277797738711039</v>
       </c>
       <c r="D37">
-        <v>0.52734375</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E37">
-        <v>0.7121022939682007</v>
+        <v>0.709696630636851</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3852,16 +3852,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5435267857142857</v>
+        <v>0.53125</v>
       </c>
       <c r="C38">
-        <v>0.7088379859924316</v>
+        <v>0.7174692392349243</v>
       </c>
       <c r="D38">
-        <v>0.546875</v>
+        <v>0.5338541666666666</v>
       </c>
       <c r="E38">
-        <v>0.7106892317533493</v>
+        <v>0.7082478304704031</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3869,16 +3869,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.5479910714285714</v>
+        <v>0.521875</v>
       </c>
       <c r="C39">
-        <v>0.7071566666875567</v>
+        <v>0.7144071340560914</v>
       </c>
       <c r="D39">
-        <v>0.5390625</v>
+        <v>0.5625</v>
       </c>
       <c r="E39">
-        <v>0.7144006639719009</v>
+        <v>0.7077093521753947</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3886,16 +3886,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5479910714285714</v>
+        <v>0.5354166666666667</v>
       </c>
       <c r="C40">
-        <v>0.7076037398406437</v>
+        <v>0.7207909822463989</v>
       </c>
       <c r="D40">
-        <v>0.52734375</v>
+        <v>0.546875</v>
       </c>
       <c r="E40">
-        <v>0.711925283074379</v>
+        <v>0.7079450984795889</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3903,16 +3903,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5502232142857143</v>
+        <v>0.521875</v>
       </c>
       <c r="C41">
-        <v>0.7069869296891349</v>
+        <v>0.7167302290598552</v>
       </c>
       <c r="D41">
-        <v>0.5390625</v>
+        <v>0.546875</v>
       </c>
       <c r="E41">
-        <v>0.7107249647378922</v>
+        <v>0.7084907690684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>